<commit_message>
we did a bayes!
</commit_message>
<xml_diff>
--- a/TravisRollsDataset.xlsx
+++ b/TravisRollsDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Bayesian-Adventure-Zone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D07DA08-4D88-4E68-B568-BD0E817A345C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861C0EA6-559E-4A78-A994-DB9948ECDF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="2085" windowWidth="18900" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45330" yWindow="705" windowWidth="11130" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TravisRollsDataset" sheetId="1" r:id="rId1"/>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>